<commit_message>
Started editing rng seed generator. Added more histograms
</commit_message>
<xml_diff>
--- a/matlab/REU_2022/Topic_3_Soaring/Sim_Draft_1/Code_of_Laws/AdamsLaw.xlsx
+++ b/matlab/REU_2022/Topic_3_Soaring/Sim_Draft_1/Code_of_Laws/AdamsLaw.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hombo\Documents\Github Repositories\REU_MatlabSim\matlab\REU_2022\Topic_3_Soaring\Sim_Draft_1\Code_of_Laws\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56CE87F4-6BAC-40A6-ADD2-BB3B1B56614C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0C8DE69-FFD1-479B-81F7-A8F750A71EB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="52" yWindow="0" windowWidth="13680" windowHeight="13080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -426,25 +426,25 @@
     <t>thermalSpawnRange</t>
   </si>
   <si>
+    <t>findNeighborhood_KNNInFixedRadius</t>
+  </si>
+  <si>
+    <t>Scores</t>
+  </si>
+  <si>
+    <t>How many boxes the map should be divided into</t>
+  </si>
+  <si>
+    <t>mapDivResolution</t>
+  </si>
+  <si>
+    <t>How often to check which divisions have been explored</t>
+  </si>
+  <si>
+    <t>mapDivFrameSkip</t>
+  </si>
+  <si>
     <t>agentControl_Unified</t>
-  </si>
-  <si>
-    <t>findNeighborhood_KNNInFixedRadius</t>
-  </si>
-  <si>
-    <t>Scores</t>
-  </si>
-  <si>
-    <t>How many boxes the map should be divided into</t>
-  </si>
-  <si>
-    <t>mapDivResolution</t>
-  </si>
-  <si>
-    <t>How often to check which divisions have been explored</t>
-  </si>
-  <si>
-    <t>mapDivFrameSkip</t>
   </si>
 </sst>
 </file>
@@ -775,8 +775,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="E94" sqref="E94"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="H43" sqref="H43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -853,7 +853,7 @@
         <v>7</v>
       </c>
       <c r="C8">
-        <v>40</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.45">
@@ -864,7 +864,7 @@
         <v>10</v>
       </c>
       <c r="C9">
-        <v>12</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.45">
@@ -896,7 +896,7 @@
         <v>104</v>
       </c>
       <c r="C13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.45">
@@ -904,7 +904,7 @@
         <v>105</v>
       </c>
       <c r="C14">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.45">
@@ -1075,7 +1075,7 @@
         <v>32</v>
       </c>
       <c r="C36" s="2">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
@@ -1090,7 +1090,7 @@
         <v>103</v>
       </c>
       <c r="C37">
-        <v>50</v>
+        <v>200</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.45">
@@ -1114,7 +1114,7 @@
         <v>34</v>
       </c>
       <c r="C40" s="2">
-        <v>1E-4</v>
+        <v>-1E-3</v>
       </c>
       <c r="D40" s="2"/>
       <c r="E40" s="2"/>
@@ -1130,7 +1130,7 @@
         <v>123</v>
       </c>
       <c r="C41">
-        <v>50</v>
+        <v>200</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.45">
@@ -1439,7 +1439,7 @@
         <v>107</v>
       </c>
       <c r="C79" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.45">
@@ -1592,7 +1592,7 @@
         <v>94</v>
       </c>
       <c r="C97" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.45">
@@ -1600,20 +1600,20 @@
         <v>95</v>
       </c>
       <c r="C98" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A100" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A101" t="s">
+        <v>132</v>
+      </c>
+      <c r="B101" t="s">
         <v>133</v>
-      </c>
-      <c r="B101" t="s">
-        <v>134</v>
       </c>
       <c r="C101">
         <v>10</v>
@@ -1621,10 +1621,10 @@
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A102" t="s">
+        <v>134</v>
+      </c>
+      <c r="B102" t="s">
         <v>135</v>
-      </c>
-      <c r="B102" t="s">
-        <v>136</v>
       </c>
       <c r="C102">
         <v>10</v>

</xml_diff>